<commit_message>
updates all the files in portuguese version
</commit_message>
<xml_diff>
--- a/atributos_pontos.xlsx
+++ b/atributos_pontos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos Mac\ASistemas\Projetos DS\balne_floripa_andhros\Balneabilidade\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E495C03A-2A77-4354-907A-964FBFB9595C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3F80B71-EF06-4835-BEF6-1498579548CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="0" windowWidth="29040" windowHeight="15840" xr2:uid="{2DE178BA-80BD-4EC6-8002-63069097DDAF}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2DE178BA-80BD-4EC6-8002-63069097DDAF}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -431,22 +431,22 @@
     <t>ponto</t>
   </si>
   <si>
-    <t>balneário</t>
-  </si>
-  <si>
     <t>referencia</t>
   </si>
   <si>
     <t>agua_doce</t>
   </si>
   <si>
-    <t>desembucadura_praia</t>
-  </si>
-  <si>
     <t>ponto_perto_desembocadura</t>
   </si>
   <si>
     <t>localizacao</t>
+  </si>
+  <si>
+    <t>balneario</t>
+  </si>
+  <si>
+    <t>desembocadura_praia</t>
   </si>
 </sst>
 </file>
@@ -800,19 +800,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{249956D1-DF38-4A54-8ECE-5373A976B6B8}">
   <dimension ref="A1:I88"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="6" max="6" width="14.88671875" customWidth="1"/>
+    <col min="7" max="7" width="23.88671875" customWidth="1"/>
+    <col min="8" max="8" width="30.88671875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>131</v>
       </c>
       <c r="B1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C1" t="s">
         <v>132</v>
-      </c>
-      <c r="C1" t="s">
-        <v>133</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -821,16 +828,16 @@
         <v>1</v>
       </c>
       <c r="F1" t="s">
+        <v>133</v>
+      </c>
+      <c r="G1" t="s">
+        <v>137</v>
+      </c>
+      <c r="H1" t="s">
         <v>134</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>135</v>
-      </c>
-      <c r="H1" t="s">
-        <v>136</v>
-      </c>
-      <c r="I1" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">

</xml_diff>